<commit_message>
Update dashboard, gauging, and field entry features
</commit_message>
<xml_diff>
--- a/Gauging Log.xlsx
+++ b/Gauging Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisRodriguez\Desktop\Cursor\Tepui Ventures Field Production App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9AE102-3E40-4528-9708-92F3709E364F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6FACC0-39D4-43A4-B7A9-999437810F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="904" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="904" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="112225" sheetId="6" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="182">
   <si>
     <t>Tank Factor</t>
   </si>
@@ -1093,8 +1093,8 @@
   <dimension ref="A1:AA999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -5653,8 +5653,8 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -5707,7 +5707,9 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="15">
+        <v>45992</v>
+      </c>
       <c r="C2" s="16"/>
       <c r="D2" s="18" t="str">
         <f>'112225'!D2</f>
@@ -5909,7 +5911,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="15">
+        <v>45992</v>
+      </c>
       <c r="C9" s="16"/>
       <c r="D9" s="18" t="str">
         <f>'112225'!D9</f>
@@ -5991,7 +5995,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="15">
+        <v>45992</v>
+      </c>
       <c r="C12" s="16"/>
       <c r="D12" s="18" t="str">
         <f>'112225'!D12</f>
@@ -6459,7 +6465,9 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="15"/>
+      <c r="B28" s="15">
+        <v>45992</v>
+      </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18" t="s">
         <v>179</v>
@@ -6478,7 +6486,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="15">
+        <v>45992</v>
+      </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18" t="s">
         <v>77</v>
@@ -6497,7 +6507,9 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="15"/>
+      <c r="B30" s="15">
+        <v>45992</v>
+      </c>
       <c r="C30" s="18"/>
       <c r="D30" s="37" t="s">
         <v>1</v>
@@ -6516,7 +6528,9 @@
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="15">
+        <v>45992</v>
+      </c>
       <c r="C31" s="18"/>
       <c r="D31" t="s">
         <v>180</v>
@@ -6535,7 +6549,9 @@
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="15"/>
+      <c r="B32" s="15">
+        <v>45992</v>
+      </c>
       <c r="C32" s="18"/>
       <c r="D32" s="2" t="s">
         <v>28</v>
@@ -6669,8 +6685,8 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -7073,9 +7089,8 @@
         <v>45993</v>
       </c>
       <c r="C12" s="16"/>
-      <c r="D12" s="18" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D12" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18">
@@ -7889,8 +7904,8 @@
   </sheetPr>
   <dimension ref="A1:M998"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -8284,9 +8299,8 @@
         <v>45994</v>
       </c>
       <c r="C12" s="21"/>
-      <c r="D12" s="22" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D12" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -15745,8 +15759,8 @@
   </sheetPr>
   <dimension ref="A1:M998"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -16189,9 +16203,8 @@
       <c r="C12" s="21">
         <v>0.46180555555555558</v>
       </c>
-      <c r="D12" s="22" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D12" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="E12" s="18">
         <v>1</v>
@@ -23724,8 +23737,8 @@
   </sheetPr>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -24096,9 +24109,8 @@
         <v>45996</v>
       </c>
       <c r="C12" s="21"/>
-      <c r="D12" s="22" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D12" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -24615,7 +24627,9 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="33"/>
+      <c r="B28" s="33">
+        <v>45996</v>
+      </c>
       <c r="C28" s="24"/>
       <c r="D28" s="18" t="s">
         <v>179</v>
@@ -24636,7 +24650,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="33"/>
+      <c r="B29" s="33">
+        <v>45996</v>
+      </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22" t="s">
         <v>77</v>
@@ -24657,7 +24673,9 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="33"/>
+      <c r="B30" s="33">
+        <v>45996</v>
+      </c>
       <c r="C30" s="24"/>
       <c r="D30" s="22" t="s">
         <v>140</v>
@@ -24701,7 +24719,9 @@
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="33"/>
+      <c r="B32" s="33">
+        <v>45996</v>
+      </c>
       <c r="C32" s="24"/>
       <c r="D32" s="22" t="s">
         <v>14</v>
@@ -24815,8 +24835,8 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -25249,9 +25269,8 @@
         <v>45997</v>
       </c>
       <c r="C12" s="21"/>
-      <c r="D12" s="22" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D12" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="E12" s="18">
         <v>1</v>
@@ -25862,7 +25881,9 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="33"/>
+      <c r="B28" s="33">
+        <v>45997</v>
+      </c>
       <c r="C28" s="24"/>
       <c r="D28" s="18" t="s">
         <v>179</v>
@@ -25883,7 +25904,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="33"/>
+      <c r="B29" s="33">
+        <v>45997</v>
+      </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22" t="s">
         <v>77</v>
@@ -25904,7 +25927,9 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="33"/>
+      <c r="B30" s="33">
+        <v>45997</v>
+      </c>
       <c r="C30" s="24"/>
       <c r="D30" s="22" t="s">
         <v>140</v>
@@ -25948,7 +25973,9 @@
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="33"/>
+      <c r="B32" s="33">
+        <v>45997</v>
+      </c>
       <c r="C32" s="24"/>
       <c r="D32" s="22" t="s">
         <v>14</v>
@@ -26062,8 +26089,8 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -26440,9 +26467,8 @@
         <v>45998</v>
       </c>
       <c r="C12" s="21"/>
-      <c r="D12" s="22" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D12" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -26975,7 +27001,9 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="33"/>
+      <c r="B28" s="33">
+        <v>45998</v>
+      </c>
       <c r="C28" s="24"/>
       <c r="D28" s="18" t="s">
         <v>179</v>
@@ -26996,7 +27024,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="33"/>
+      <c r="B29" s="33">
+        <v>45998</v>
+      </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22" t="s">
         <v>77</v>
@@ -27017,7 +27047,9 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="33"/>
+      <c r="B30" s="33">
+        <v>45998</v>
+      </c>
       <c r="C30" s="24"/>
       <c r="D30" s="22" t="s">
         <v>140</v>
@@ -27038,7 +27070,9 @@
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="33"/>
+      <c r="B31" s="33">
+        <v>45998</v>
+      </c>
       <c r="C31" s="24"/>
       <c r="D31" s="22" t="s">
         <v>28</v>
@@ -27059,7 +27093,9 @@
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="33"/>
+      <c r="B32" s="33">
+        <v>45998</v>
+      </c>
       <c r="C32" s="24"/>
       <c r="D32" s="22" t="s">
         <v>14</v>
@@ -27162,6 +27198,7 @@
     <mergeCell ref="E8:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -27172,8 +27209,8 @@
   </sheetPr>
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -27608,9 +27645,8 @@
         <v>45999</v>
       </c>
       <c r="C12" s="21"/>
-      <c r="D12" s="22" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D12" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="E12" s="18">
         <v>1</v>
@@ -28426,9 +28462,9 @@
   </sheetPr>
   <dimension ref="A1:M999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -28815,9 +28851,8 @@
         <v>46000</v>
       </c>
       <c r="C12" s="21"/>
-      <c r="D12" s="22" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D12" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -29237,7 +29272,9 @@
       <c r="A25" s="20">
         <v>24</v>
       </c>
-      <c r="B25" s="33"/>
+      <c r="B25" s="33">
+        <v>46000</v>
+      </c>
       <c r="C25" s="21"/>
       <c r="D25" s="22" t="s">
         <v>22</v>
@@ -29256,7 +29293,9 @@
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="33"/>
+      <c r="B26" s="33">
+        <v>46000</v>
+      </c>
       <c r="C26" s="21"/>
       <c r="D26" s="22" t="s">
         <v>25</v>
@@ -29275,7 +29314,9 @@
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="33"/>
+      <c r="B27" s="33">
+        <v>46000</v>
+      </c>
       <c r="C27" s="47"/>
       <c r="D27" s="22" t="s">
         <v>27</v>
@@ -29346,7 +29387,9 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="33"/>
+      <c r="B30" s="33">
+        <v>46000</v>
+      </c>
       <c r="C30" s="24"/>
       <c r="D30" s="22" t="s">
         <v>140</v>
@@ -29367,7 +29410,9 @@
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="33"/>
+      <c r="B31" s="33">
+        <v>46000</v>
+      </c>
       <c r="C31" s="24"/>
       <c r="D31" s="22" t="s">
         <v>28</v>
@@ -29388,7 +29433,9 @@
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="33"/>
+      <c r="B32" s="33">
+        <v>46000</v>
+      </c>
       <c r="C32" s="24"/>
       <c r="D32" s="22" t="s">
         <v>14</v>
@@ -32389,8 +32436,8 @@
   <dimension ref="A1:AA999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -36886,8 +36933,8 @@
   <dimension ref="A1:AA999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -41793,8 +41840,8 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -43661,8 +43708,8 @@
   <dimension ref="A1:AA999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -44739,7 +44786,9 @@
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" s="15">
+        <v>45987</v>
+      </c>
       <c r="C27" s="29"/>
       <c r="D27" s="18" t="str">
         <f>'112225'!D27</f>
@@ -44792,7 +44841,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="15">
+        <v>45987</v>
+      </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18" t="s">
         <v>77</v>
@@ -48341,7 +48392,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -53014,9 +53065,9 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -54086,7 +54137,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="15">
+        <v>45989</v>
+      </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18" t="s">
         <v>77</v>
@@ -54292,8 +54345,8 @@
   <dimension ref="A1:M999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -54346,7 +54399,9 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="15">
+        <v>45990</v>
+      </c>
       <c r="C2" s="16"/>
       <c r="D2" s="18" t="str">
         <f>'112225'!D2</f>
@@ -54370,7 +54425,9 @@
       <c r="A3" s="20">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="15">
+        <v>45990</v>
+      </c>
       <c r="C3" s="21"/>
       <c r="D3" s="18" t="str">
         <f>'112225'!D3</f>
@@ -54394,7 +54451,9 @@
       <c r="A4" s="20">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="15">
+        <v>45990</v>
+      </c>
       <c r="C4" s="21"/>
       <c r="D4" s="18" t="str">
         <f>'112225'!D4</f>
@@ -54418,7 +54477,9 @@
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="15">
+        <v>45990</v>
+      </c>
       <c r="C5" s="16"/>
       <c r="D5" s="18" t="str">
         <f>'112225'!D5</f>
@@ -54440,7 +54501,9 @@
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="15">
+        <v>45990</v>
+      </c>
       <c r="C6" s="16"/>
       <c r="D6" s="18" t="str">
         <f>'112225'!D6</f>
@@ -54464,7 +54527,9 @@
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="15">
+        <v>45990</v>
+      </c>
       <c r="C7" s="16"/>
       <c r="D7" s="18" t="str">
         <f>'112225'!D7</f>
@@ -54488,7 +54553,9 @@
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="15">
+        <v>45990</v>
+      </c>
       <c r="C8" s="16"/>
       <c r="D8" s="18" t="str">
         <f>'112225'!D8</f>
@@ -54512,7 +54579,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="15">
+        <v>45990</v>
+      </c>
       <c r="C9" s="16"/>
       <c r="D9" s="18" t="str">
         <f>'112225'!D9</f>
@@ -54536,7 +54605,9 @@
       <c r="A10" s="20">
         <v>9</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="15">
+        <v>45990</v>
+      </c>
       <c r="C10" s="21"/>
       <c r="D10" s="18" t="str">
         <f>'112225'!D10</f>
@@ -54560,7 +54631,9 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="15">
+        <v>45990</v>
+      </c>
       <c r="C11" s="16"/>
       <c r="D11" s="18" t="str">
         <f>'112225'!D11</f>
@@ -54584,7 +54657,9 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="15">
+        <v>45990</v>
+      </c>
       <c r="C12" s="16"/>
       <c r="D12" s="18" t="str">
         <f>'112225'!D12</f>
@@ -54608,7 +54683,9 @@
       <c r="A13" s="20">
         <v>12</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="15">
+        <v>45990</v>
+      </c>
       <c r="C13" s="21"/>
       <c r="D13" s="18" t="str">
         <f>'112225'!D13</f>
@@ -54632,7 +54709,9 @@
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="15">
+        <v>45990</v>
+      </c>
       <c r="C14" s="16"/>
       <c r="D14" s="18" t="str">
         <f>'112225'!D14</f>
@@ -54654,7 +54733,9 @@
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="15"/>
+      <c r="B15" s="15">
+        <v>45990</v>
+      </c>
       <c r="C15" s="16"/>
       <c r="D15" s="18" t="str">
         <f>'112225'!D15</f>
@@ -54690,7 +54771,9 @@
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="15">
+        <v>45990</v>
+      </c>
       <c r="C16" s="16"/>
       <c r="D16" s="18" t="str">
         <f>'112225'!D16</f>
@@ -54716,7 +54799,9 @@
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="15"/>
+      <c r="B17" s="15">
+        <v>45990</v>
+      </c>
       <c r="C17" s="16"/>
       <c r="D17" s="18" t="str">
         <f>'112225'!D17</f>
@@ -54742,7 +54827,9 @@
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="15">
+        <v>45990</v>
+      </c>
       <c r="C18" s="16"/>
       <c r="D18" s="18" t="str">
         <f>'112225'!D18</f>
@@ -54770,7 +54857,9 @@
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="15"/>
+      <c r="B19" s="15">
+        <v>45990</v>
+      </c>
       <c r="C19" s="16"/>
       <c r="D19" s="18" t="str">
         <f>'112225'!D19</f>
@@ -54798,7 +54887,9 @@
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="15"/>
+      <c r="B20" s="15">
+        <v>45990</v>
+      </c>
       <c r="C20" s="16"/>
       <c r="D20" s="18" t="str">
         <f>'112225'!D20</f>
@@ -54826,7 +54917,9 @@
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="15"/>
+      <c r="B21" s="15">
+        <v>45990</v>
+      </c>
       <c r="C21" s="16"/>
       <c r="D21" s="18" t="str">
         <f>'112225'!D21</f>
@@ -54854,7 +54947,9 @@
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="15"/>
+      <c r="B22" s="15">
+        <v>45990</v>
+      </c>
       <c r="C22" s="16"/>
       <c r="D22" s="18" t="str">
         <f>'112225'!D22</f>
@@ -54882,7 +54977,9 @@
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="15"/>
+      <c r="B23" s="15">
+        <v>45990</v>
+      </c>
       <c r="C23" s="16"/>
       <c r="D23" s="18" t="str">
         <f>'112225'!D23</f>
@@ -54910,7 +55007,9 @@
       <c r="A24" s="20">
         <v>23</v>
       </c>
-      <c r="B24" s="15"/>
+      <c r="B24" s="15">
+        <v>45990</v>
+      </c>
       <c r="C24" s="21"/>
       <c r="D24" s="18" t="str">
         <f>'112225'!D24</f>
@@ -54938,7 +55037,9 @@
       <c r="A25" s="20">
         <v>24</v>
       </c>
-      <c r="B25" s="15"/>
+      <c r="B25" s="15">
+        <v>45990</v>
+      </c>
       <c r="C25" s="21"/>
       <c r="D25" s="18" t="str">
         <f>'112225'!D25</f>
@@ -54966,7 +55067,9 @@
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="15"/>
+      <c r="B26" s="15">
+        <v>45990</v>
+      </c>
       <c r="C26" s="16"/>
       <c r="D26" s="18" t="str">
         <f>'112225'!D26</f>
@@ -54994,7 +55097,9 @@
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" s="15">
+        <v>45990</v>
+      </c>
       <c r="C27" s="35"/>
       <c r="D27" s="18" t="str">
         <f>'112225'!D27</f>
@@ -55016,7 +55121,9 @@
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="15"/>
+      <c r="B28" s="15">
+        <v>45990</v>
+      </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18" t="s">
         <v>179</v>
@@ -55041,7 +55148,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="15">
+        <v>45990</v>
+      </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18" t="s">
         <v>77</v>
@@ -55060,7 +55169,9 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="15"/>
+      <c r="B30" s="15">
+        <v>45990</v>
+      </c>
       <c r="C30" s="18"/>
       <c r="D30" s="37" t="s">
         <v>1</v>
@@ -55083,7 +55194,9 @@
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="15">
+        <v>45990</v>
+      </c>
       <c r="C31" s="18"/>
       <c r="D31" t="s">
         <v>180</v>
@@ -58119,8 +58232,8 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" customHeight="1"/>
@@ -58444,7 +58557,9 @@
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="15">
+        <v>45991</v>
+      </c>
       <c r="C9" s="16"/>
       <c r="D9" s="18" t="str">
         <f>'112225'!D9</f>
@@ -58616,7 +58731,9 @@
       <c r="A14" s="7">
         <v>13</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="15">
+        <v>45991</v>
+      </c>
       <c r="C14" s="16"/>
       <c r="D14" s="18" t="str">
         <f>'112225'!D14</f>
@@ -59183,7 +59300,9 @@
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="15">
+        <v>45991</v>
+      </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18" t="s">
         <v>77</v>
@@ -59206,7 +59325,9 @@
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="15"/>
+      <c r="B30" s="15">
+        <v>45991</v>
+      </c>
       <c r="C30" s="18"/>
       <c r="D30" s="37" t="s">
         <v>1</v>
@@ -59229,7 +59350,9 @@
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="15">
+        <v>45991</v>
+      </c>
       <c r="C31" s="18"/>
       <c r="D31" t="s">
         <v>180</v>

</xml_diff>